<commit_message>
update public: 2019 end
</commit_message>
<xml_diff>
--- a/data/Bosses.xlsx
+++ b/data/Bosses.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20702"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip Masic\OneDrive\Documents\Code\DiscordJME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_B9A2815CB4EAE93A742E805192B1FA30A957D96E" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179020"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,18 +27,30 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
+    <t>Boss</t>
+  </si>
+  <si>
     <t>Tier</t>
   </si>
   <si>
-    <t>Boss</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
     <t>magikarp</t>
   </si>
   <si>
+    <t>ivysaur</t>
+  </si>
+  <si>
+    <t>charmeleon</t>
+  </si>
+  <si>
+    <t>wartortle</t>
+  </si>
+  <si>
+    <t>metapod</t>
+  </si>
+  <si>
     <t>bayleef</t>
   </si>
   <si>
@@ -47,6 +60,27 @@
     <t>croconaw</t>
   </si>
   <si>
+    <t>sandslash</t>
+  </si>
+  <si>
+    <t>tentacruel</t>
+  </si>
+  <si>
+    <t>magneton</t>
+  </si>
+  <si>
+    <t>cloyster</t>
+  </si>
+  <si>
+    <t>marowak</t>
+  </si>
+  <si>
+    <t>sableye</t>
+  </si>
+  <si>
+    <t>mawile</t>
+  </si>
+  <si>
     <t>muk</t>
   </si>
   <si>
@@ -62,18 +96,30 @@
     <t>magmar</t>
   </si>
   <si>
+    <t>alakazam</t>
+  </si>
+  <si>
+    <t>machamp</t>
+  </si>
+  <si>
+    <t>gengar</t>
+  </si>
+  <si>
+    <t>ninetales</t>
+  </si>
+  <si>
+    <t>scyther</t>
+  </si>
+  <si>
+    <t>porygon</t>
+  </si>
+  <si>
+    <t>omastar</t>
+  </si>
+  <si>
     <t>arcanine</t>
   </si>
   <si>
-    <t>alakazam</t>
-  </si>
-  <si>
-    <t>machamp</t>
-  </si>
-  <si>
-    <t>gengar</t>
-  </si>
-  <si>
     <t>vaporeon</t>
   </si>
   <si>
@@ -83,6 +129,33 @@
     <t>flareon</t>
   </si>
   <si>
+    <t>lapras</t>
+  </si>
+  <si>
+    <t>snorlax</t>
+  </si>
+  <si>
+    <t>tyranitar</t>
+  </si>
+  <si>
+    <t>nidoqueen</t>
+  </si>
+  <si>
+    <t>nidoking</t>
+  </si>
+  <si>
+    <t>poliwrath</t>
+  </si>
+  <si>
+    <t>victreebel</t>
+  </si>
+  <si>
+    <t>golem</t>
+  </si>
+  <si>
+    <t>absol</t>
+  </si>
+  <si>
     <t>venusaur</t>
   </si>
   <si>
@@ -95,70 +168,16 @@
     <t>rhydon</t>
   </si>
   <si>
-    <t>lapras</t>
-  </si>
-  <si>
-    <t>snorlax</t>
-  </si>
-  <si>
-    <t>tyranitar</t>
-  </si>
-  <si>
-    <t>ivysaur</t>
-  </si>
-  <si>
-    <t>charmeleon</t>
-  </si>
-  <si>
-    <t>wartortle</t>
-  </si>
-  <si>
-    <t>metapod</t>
-  </si>
-  <si>
-    <t>sandslash</t>
-  </si>
-  <si>
-    <t>tentacruel</t>
-  </si>
-  <si>
-    <t>magneton</t>
-  </si>
-  <si>
-    <t>cloyster</t>
-  </si>
-  <si>
-    <t>marowak</t>
-  </si>
-  <si>
-    <t>sableye</t>
-  </si>
-  <si>
-    <t>ninetales</t>
-  </si>
-  <si>
-    <t>scyther</t>
-  </si>
-  <si>
-    <t>porygon</t>
-  </si>
-  <si>
-    <t>omastar</t>
-  </si>
-  <si>
-    <t>nidoqueen</t>
-  </si>
-  <si>
-    <t>nidoking</t>
-  </si>
-  <si>
-    <t>poliwrath</t>
-  </si>
-  <si>
-    <t>victreebel</t>
-  </si>
-  <si>
-    <t>golem</t>
+    <t>mewtwo</t>
+  </si>
+  <si>
+    <t>groudon</t>
+  </si>
+  <si>
+    <t>kyogre</t>
+  </si>
+  <si>
+    <t>rayquaza</t>
   </si>
   <si>
     <t>articuno</t>
@@ -173,9 +192,6 @@
     <t>lugia</t>
   </si>
   <si>
-    <t>mewtwo</t>
-  </si>
-  <si>
     <t>raikou</t>
   </si>
   <si>
@@ -192,28 +208,13 @@
   </si>
   <si>
     <t>celebi</t>
-  </si>
-  <si>
-    <t>absol</t>
-  </si>
-  <si>
-    <t>mawile</t>
-  </si>
-  <si>
-    <t>groudon</t>
-  </si>
-  <si>
-    <t>kyogre</t>
-  </si>
-  <si>
-    <t>rayquaza</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -597,30 +598,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="16384" width="17.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -631,9 +632,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -642,9 +643,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -653,9 +654,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -664,9 +665,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -675,9 +676,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -686,9 +687,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -697,9 +698,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -708,9 +709,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
@@ -719,9 +720,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
@@ -730,9 +731,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
@@ -741,9 +742,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
@@ -752,9 +753,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
@@ -763,9 +764,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
@@ -774,9 +775,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
@@ -785,9 +786,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -796,9 +797,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
@@ -807,9 +808,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
@@ -818,9 +819,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
@@ -829,9 +830,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
@@ -840,9 +841,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -851,9 +852,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" s="4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1">
         <v>3</v>
@@ -862,9 +863,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1">
         <v>3</v>
@@ -873,9 +874,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1">
         <v>3</v>
@@ -884,9 +885,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1">
         <v>3</v>
@@ -895,9 +896,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1">
         <v>3</v>
@@ -906,9 +907,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" s="4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1">
         <v>3</v>
@@ -917,9 +918,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" s="4" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1">
         <v>3</v>
@@ -928,9 +929,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" s="4" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
@@ -939,9 +940,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" s="4" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1">
         <v>3</v>
@@ -950,9 +951,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" s="4" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B32" s="1">
         <v>3</v>
@@ -961,9 +962,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1">
         <v>4</v>
@@ -972,9 +973,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" s="5" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1">
         <v>4</v>
@@ -983,9 +984,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1">
         <v>4</v>
@@ -994,262 +995,262 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="1">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="1">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="1">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="1">
-        <v>4</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="B39" s="1">
+        <v>4</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="1">
-        <v>4</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="B40" s="1">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="1">
-        <v>4</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="B41" s="1">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="1">
-        <v>4</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="B42" s="1">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="1">
-        <v>4</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="B43" s="1">
+        <v>4</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="1">
+        <v>4</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="1">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="1">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="1">
+        <v>5</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="1">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="1">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="1">
+        <v>5</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="1">
+        <v>5</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="1">
+        <v>5</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="1">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="1">
+        <v>5</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="1">
-        <v>4</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="1">
-        <v>4</v>
-      </c>
-      <c r="C42" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="1">
-        <v>4</v>
-      </c>
-      <c r="C43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B44" s="1">
-        <v>4</v>
-      </c>
-      <c r="C44" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="1">
-        <v>4</v>
-      </c>
-      <c r="C45" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="1">
-        <v>5</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="B55" s="1">
+        <v>5</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="1">
+        <v>5</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="1">
-        <v>5</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="B57" s="1">
+        <v>5</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="1">
-        <v>5</v>
-      </c>
-      <c r="C48" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="B58" s="1">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B49" s="1">
-        <v>5</v>
-      </c>
-      <c r="C49" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="1">
-        <v>5</v>
-      </c>
-      <c r="C50" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51" s="1">
-        <v>5</v>
-      </c>
-      <c r="C51" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B52" s="1">
-        <v>5</v>
-      </c>
-      <c r="C52" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="1">
-        <v>5</v>
-      </c>
-      <c r="C53" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="1">
-        <v>5</v>
-      </c>
-      <c r="C54" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B55" s="1">
-        <v>5</v>
-      </c>
-      <c r="C55" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" s="1">
-        <v>5</v>
-      </c>
-      <c r="C56" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="1">
-        <v>5</v>
-      </c>
-      <c r="C57" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" s="1">
-        <v>5</v>
-      </c>
-      <c r="C58" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="B59" s="1">
         <v>5</v>

</xml_diff>